<commit_message>
filter nan libro-opinión, assign order of the columns
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -400,22 +400,22 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>Media</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Cuasidesviación</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Mediana</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
           <t>Moda</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Media</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Cuasidesviación</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Mediana</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
@@ -454,13 +454,13 @@
         <v>173</v>
       </c>
       <c r="C2" s="1" t="n">
+        <v>5.283236994219653</v>
+      </c>
+      <c r="D2" s="1" t="n">
+        <v>1.213110041412962</v>
+      </c>
+      <c r="E2" s="1" t="n">
         <v>6</v>
-      </c>
-      <c r="D2" s="1" t="n">
-        <v>5.283236994219653</v>
-      </c>
-      <c r="E2" s="1" t="n">
-        <v>1.213110041412962</v>
       </c>
       <c r="F2" s="1" t="n">
         <v>6</v>
@@ -606,13 +606,13 @@
         <v>63</v>
       </c>
       <c r="C8" s="1" t="n">
+        <v>5.682539682539683</v>
+      </c>
+      <c r="D8" s="1" t="n">
+        <v>0.8948850498428026</v>
+      </c>
+      <c r="E8" s="1" t="n">
         <v>6</v>
-      </c>
-      <c r="D8" s="1" t="n">
-        <v>5.682539682539683</v>
-      </c>
-      <c r="E8" s="1" t="n">
-        <v>0.8948850498428026</v>
       </c>
       <c r="F8" s="1" t="n">
         <v>6</v>

</xml_diff>

<commit_message>
Especialty Grouping and sort by count-rate
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -379,7 +379,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K13"/>
+  <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -390,55 +390,60 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>Especialidad</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>Libro</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Número de Valoraciones</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Media</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Cuasidesviación</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Mediana</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Moda</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Opinión del 1 al 6</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>fi</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>hi</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Fi</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>Hi</t>
         </is>
@@ -447,37 +452,42 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
+          <t>Eje Transversal</t>
+        </is>
+      </c>
+      <c r="B2" s="1" t="inlineStr">
+        <is>
           <t>Libro 68</t>
         </is>
       </c>
-      <c r="B2" s="1" t="n">
+      <c r="C2" s="1" t="n">
         <v>173</v>
       </c>
-      <c r="C2" s="1" t="n">
+      <c r="D2" s="1" t="n">
         <v>5.283236994219653</v>
       </c>
-      <c r="D2" s="1" t="n">
+      <c r="E2" s="1" t="n">
         <v>1.213110041412962</v>
-      </c>
-      <c r="E2" s="1" t="n">
-        <v>6</v>
       </c>
       <c r="F2" s="1" t="n">
         <v>6</v>
       </c>
       <c r="G2" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="H2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="H2" t="n">
+      <c r="I2" t="n">
         <v>5</v>
       </c>
-      <c r="I2" t="n">
+      <c r="J2" t="n">
         <v>2.890173410404624</v>
       </c>
-      <c r="J2" t="n">
+      <c r="K2" t="n">
         <v>5</v>
       </c>
-      <c r="K2" t="n">
+      <c r="L2" t="n">
         <v>2.890173410404624</v>
       </c>
     </row>
@@ -488,19 +498,20 @@
       <c r="D3" s="1" t="n"/>
       <c r="E3" s="1" t="n"/>
       <c r="F3" s="1" t="n"/>
-      <c r="G3" s="1" t="n">
+      <c r="G3" s="1" t="n"/>
+      <c r="H3" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="H3" t="n">
+      <c r="I3" t="n">
         <v>2</v>
       </c>
-      <c r="I3" t="n">
+      <c r="J3" t="n">
         <v>1.15606936416185</v>
       </c>
-      <c r="J3" t="n">
+      <c r="K3" t="n">
         <v>7</v>
       </c>
-      <c r="K3" t="n">
+      <c r="L3" t="n">
         <v>4.046242774566474</v>
       </c>
     </row>
@@ -511,19 +522,20 @@
       <c r="D4" s="1" t="n"/>
       <c r="E4" s="1" t="n"/>
       <c r="F4" s="1" t="n"/>
-      <c r="G4" s="1" t="n">
+      <c r="G4" s="1" t="n"/>
+      <c r="H4" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="H4" t="n">
+      <c r="I4" t="n">
         <v>12</v>
       </c>
-      <c r="I4" t="n">
+      <c r="J4" t="n">
         <v>6.936416184971097</v>
       </c>
-      <c r="J4" t="n">
+      <c r="K4" t="n">
         <v>19</v>
       </c>
-      <c r="K4" t="n">
+      <c r="L4" t="n">
         <v>10.98265895953757</v>
       </c>
     </row>
@@ -534,19 +546,20 @@
       <c r="D5" s="1" t="n"/>
       <c r="E5" s="1" t="n"/>
       <c r="F5" s="1" t="n"/>
-      <c r="G5" s="1" t="n">
+      <c r="G5" s="1" t="n"/>
+      <c r="H5" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="H5" t="n">
+      <c r="I5" t="n">
         <v>11</v>
       </c>
-      <c r="I5" t="n">
+      <c r="J5" t="n">
         <v>6.358381502890173</v>
       </c>
-      <c r="J5" t="n">
+      <c r="K5" t="n">
         <v>30</v>
       </c>
-      <c r="K5" t="n">
+      <c r="L5" t="n">
         <v>17.34104046242775</v>
       </c>
     </row>
@@ -557,19 +570,20 @@
       <c r="D6" s="1" t="n"/>
       <c r="E6" s="1" t="n"/>
       <c r="F6" s="1" t="n"/>
-      <c r="G6" s="1" t="n">
+      <c r="G6" s="1" t="n"/>
+      <c r="H6" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="H6" t="n">
+      <c r="I6" t="n">
         <v>33</v>
       </c>
-      <c r="I6" t="n">
+      <c r="J6" t="n">
         <v>19.07514450867052</v>
       </c>
-      <c r="J6" t="n">
+      <c r="K6" t="n">
         <v>63</v>
       </c>
-      <c r="K6" t="n">
+      <c r="L6" t="n">
         <v>36.41618497109826</v>
       </c>
     </row>
@@ -580,56 +594,58 @@
       <c r="D7" s="1" t="n"/>
       <c r="E7" s="1" t="n"/>
       <c r="F7" s="1" t="n"/>
-      <c r="G7" s="1" t="n">
+      <c r="G7" s="1" t="n"/>
+      <c r="H7" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="H7" t="n">
+      <c r="I7" t="n">
         <v>110</v>
       </c>
-      <c r="I7" t="n">
+      <c r="J7" t="n">
         <v>63.58381502890174</v>
       </c>
-      <c r="J7" t="n">
+      <c r="K7" t="n">
         <v>173</v>
       </c>
-      <c r="K7" t="n">
+      <c r="L7" t="n">
         <v>100</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="inlineStr">
+      <c r="A8" s="1" t="n"/>
+      <c r="B8" s="1" t="inlineStr">
         <is>
           <t>Libro 69</t>
         </is>
       </c>
-      <c r="B8" s="1" t="n">
+      <c r="C8" s="1" t="n">
         <v>63</v>
       </c>
-      <c r="C8" s="1" t="n">
+      <c r="D8" s="1" t="n">
         <v>5.682539682539683</v>
       </c>
-      <c r="D8" s="1" t="n">
+      <c r="E8" s="1" t="n">
         <v>0.8948850498428026</v>
-      </c>
-      <c r="E8" s="1" t="n">
-        <v>6</v>
       </c>
       <c r="F8" s="1" t="n">
         <v>6</v>
       </c>
       <c r="G8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="H8" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="H8" t="n">
+      <c r="I8" t="n">
         <v>1</v>
       </c>
-      <c r="I8" t="n">
+      <c r="J8" t="n">
         <v>1.587301587301587</v>
       </c>
-      <c r="J8" t="n">
+      <c r="K8" t="n">
         <v>1</v>
       </c>
-      <c r="K8" t="n">
+      <c r="L8" t="n">
         <v>1.587301587301587</v>
       </c>
     </row>
@@ -640,11 +656,9 @@
       <c r="D9" s="1" t="n"/>
       <c r="E9" s="1" t="n"/>
       <c r="F9" s="1" t="n"/>
-      <c r="G9" s="1" t="n">
+      <c r="G9" s="1" t="n"/>
+      <c r="H9" s="1" t="n">
         <v>2</v>
-      </c>
-      <c r="H9" t="n">
-        <v>0</v>
       </c>
       <c r="I9" t="n">
         <v>0</v>
@@ -653,6 +667,9 @@
         <v>0</v>
       </c>
       <c r="K9" t="n">
+        <v>0</v>
+      </c>
+      <c r="L9" t="n">
         <v>0</v>
       </c>
     </row>
@@ -663,19 +680,20 @@
       <c r="D10" s="1" t="n"/>
       <c r="E10" s="1" t="n"/>
       <c r="F10" s="1" t="n"/>
-      <c r="G10" s="1" t="n">
+      <c r="G10" s="1" t="n"/>
+      <c r="H10" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="H10" t="n">
+      <c r="I10" t="n">
         <v>1</v>
       </c>
-      <c r="I10" t="n">
+      <c r="J10" t="n">
         <v>1.587301587301587</v>
       </c>
-      <c r="J10" t="n">
+      <c r="K10" t="n">
         <v>2</v>
       </c>
-      <c r="K10" t="n">
+      <c r="L10" t="n">
         <v>3.174603174603174</v>
       </c>
     </row>
@@ -686,19 +704,20 @@
       <c r="D11" s="1" t="n"/>
       <c r="E11" s="1" t="n"/>
       <c r="F11" s="1" t="n"/>
-      <c r="G11" s="1" t="n">
+      <c r="G11" s="1" t="n"/>
+      <c r="H11" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="H11" t="n">
+      <c r="I11" t="n">
         <v>5</v>
       </c>
-      <c r="I11" t="n">
+      <c r="J11" t="n">
         <v>7.936507936507936</v>
       </c>
-      <c r="J11" t="n">
+      <c r="K11" t="n">
         <v>7</v>
       </c>
-      <c r="K11" t="n">
+      <c r="L11" t="n">
         <v>11.11111111111111</v>
       </c>
     </row>
@@ -709,19 +728,20 @@
       <c r="D12" s="1" t="n"/>
       <c r="E12" s="1" t="n"/>
       <c r="F12" s="1" t="n"/>
-      <c r="G12" s="1" t="n">
+      <c r="G12" s="1" t="n"/>
+      <c r="H12" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="H12" t="n">
+      <c r="I12" t="n">
         <v>2</v>
       </c>
-      <c r="I12" t="n">
+      <c r="J12" t="n">
         <v>3.174603174603174</v>
       </c>
-      <c r="J12" t="n">
+      <c r="K12" t="n">
         <v>9</v>
       </c>
-      <c r="K12" t="n">
+      <c r="L12" t="n">
         <v>14.28571428571428</v>
       </c>
     </row>
@@ -732,26 +752,26 @@
       <c r="D13" s="1" t="n"/>
       <c r="E13" s="1" t="n"/>
       <c r="F13" s="1" t="n"/>
-      <c r="G13" s="1" t="n">
+      <c r="G13" s="1" t="n"/>
+      <c r="H13" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="H13" t="n">
+      <c r="I13" t="n">
         <v>54</v>
       </c>
-      <c r="I13" t="n">
+      <c r="J13" t="n">
         <v>85.71428571428571</v>
       </c>
-      <c r="J13" t="n">
+      <c r="K13" t="n">
         <v>63</v>
       </c>
-      <c r="K13" t="n">
+      <c r="L13" t="n">
         <v>100</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="12">
-    <mergeCell ref="A2:A7"/>
-    <mergeCell ref="A8:A13"/>
+  <mergeCells count="13">
+    <mergeCell ref="A2:A13"/>
     <mergeCell ref="B2:B7"/>
     <mergeCell ref="B8:B13"/>
     <mergeCell ref="C2:C7"/>
@@ -762,6 +782,8 @@
     <mergeCell ref="E8:E13"/>
     <mergeCell ref="F2:F7"/>
     <mergeCell ref="F8:F13"/>
+    <mergeCell ref="G2:G7"/>
+    <mergeCell ref="G8:G13"/>
   </mergeCells>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
filtering non dispersed data
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -7,7 +7,8 @@
     <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="tabla de datos dispersos" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -379,6 +380,24 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
using moment kurtosis and skew
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -398,7 +398,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R13"/>
+  <dimension ref="A1:Q13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -419,7 +419,7 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Número de Valoraciones</t>
+          <t>Nº Valoraciones</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
@@ -434,7 +434,7 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Curtosis</t>
+          <t>Cu</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
@@ -459,40 +459,35 @@
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>Rango Intercuartil</t>
+          <t>Q3-Q1</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>P(90) - P(10)</t>
+          <t>Moda</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>Moda</t>
+          <t>Opinión del 1 al 6</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t>Opinión del 1 al 6</t>
+          <t>fi</t>
         </is>
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
-          <t>fi</t>
+          <t>hi</t>
         </is>
       </c>
       <c r="P1" s="1" t="inlineStr">
         <is>
-          <t>hi</t>
+          <t>Fi</t>
         </is>
       </c>
       <c r="Q1" s="1" t="inlineStr">
-        <is>
-          <t>Fi</t>
-        </is>
-      </c>
-      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>Hi</t>
         </is>
@@ -519,10 +514,10 @@
         <v>1.213110041412963</v>
       </c>
       <c r="F2" s="1" t="n">
-        <v>0.1666666666666667</v>
+        <v>3.341999482007184</v>
       </c>
       <c r="G2" s="1" t="n">
-        <v>-1.772542427261178</v>
+        <v>-1.943931833238586</v>
       </c>
       <c r="H2" s="1" t="n">
         <v>5</v>
@@ -537,24 +532,21 @@
         <v>1</v>
       </c>
       <c r="L2" s="1" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="M2" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="N2" s="1" t="n">
         <v>1</v>
       </c>
+      <c r="N2" t="n">
+        <v>5</v>
+      </c>
       <c r="O2" t="n">
+        <v>2.890173410404624</v>
+      </c>
+      <c r="P2" t="n">
         <v>5</v>
       </c>
-      <c r="P2" t="n">
-        <v>2.890173410404624</v>
-      </c>
       <c r="Q2" t="n">
-        <v>5</v>
-      </c>
-      <c r="R2" t="n">
         <v>2.890173410404624</v>
       </c>
     </row>
@@ -571,20 +563,19 @@
       <c r="J3" s="1" t="n"/>
       <c r="K3" s="1" t="n"/>
       <c r="L3" s="1" t="n"/>
-      <c r="M3" s="1" t="n"/>
-      <c r="N3" s="1" t="n">
+      <c r="M3" s="1" t="n">
         <v>2</v>
       </c>
+      <c r="N3" t="n">
+        <v>2</v>
+      </c>
       <c r="O3" t="n">
-        <v>2</v>
+        <v>1.15606936416185</v>
       </c>
       <c r="P3" t="n">
-        <v>1.15606936416185</v>
+        <v>7</v>
       </c>
       <c r="Q3" t="n">
-        <v>7</v>
-      </c>
-      <c r="R3" t="n">
         <v>4.046242774566474</v>
       </c>
     </row>
@@ -601,20 +592,19 @@
       <c r="J4" s="1" t="n"/>
       <c r="K4" s="1" t="n"/>
       <c r="L4" s="1" t="n"/>
-      <c r="M4" s="1" t="n"/>
-      <c r="N4" s="1" t="n">
+      <c r="M4" s="1" t="n">
         <v>3</v>
       </c>
+      <c r="N4" t="n">
+        <v>12</v>
+      </c>
       <c r="O4" t="n">
-        <v>12</v>
+        <v>6.936416184971097</v>
       </c>
       <c r="P4" t="n">
-        <v>6.936416184971097</v>
+        <v>19</v>
       </c>
       <c r="Q4" t="n">
-        <v>19</v>
-      </c>
-      <c r="R4" t="n">
         <v>10.98265895953757</v>
       </c>
     </row>
@@ -631,20 +621,19 @@
       <c r="J5" s="1" t="n"/>
       <c r="K5" s="1" t="n"/>
       <c r="L5" s="1" t="n"/>
-      <c r="M5" s="1" t="n"/>
-      <c r="N5" s="1" t="n">
+      <c r="M5" s="1" t="n">
         <v>4</v>
       </c>
+      <c r="N5" t="n">
+        <v>11</v>
+      </c>
       <c r="O5" t="n">
-        <v>11</v>
+        <v>6.358381502890173</v>
       </c>
       <c r="P5" t="n">
-        <v>6.358381502890173</v>
+        <v>30</v>
       </c>
       <c r="Q5" t="n">
-        <v>30</v>
-      </c>
-      <c r="R5" t="n">
         <v>17.34104046242775</v>
       </c>
     </row>
@@ -661,20 +650,19 @@
       <c r="J6" s="1" t="n"/>
       <c r="K6" s="1" t="n"/>
       <c r="L6" s="1" t="n"/>
-      <c r="M6" s="1" t="n"/>
-      <c r="N6" s="1" t="n">
+      <c r="M6" s="1" t="n">
         <v>5</v>
       </c>
+      <c r="N6" t="n">
+        <v>33</v>
+      </c>
       <c r="O6" t="n">
-        <v>33</v>
+        <v>19.07514450867052</v>
       </c>
       <c r="P6" t="n">
-        <v>19.07514450867052</v>
+        <v>63</v>
       </c>
       <c r="Q6" t="n">
-        <v>63</v>
-      </c>
-      <c r="R6" t="n">
         <v>36.41618497109826</v>
       </c>
     </row>
@@ -691,20 +679,19 @@
       <c r="J7" s="1" t="n"/>
       <c r="K7" s="1" t="n"/>
       <c r="L7" s="1" t="n"/>
-      <c r="M7" s="1" t="n"/>
-      <c r="N7" s="1" t="n">
+      <c r="M7" s="1" t="n">
         <v>6</v>
       </c>
+      <c r="N7" t="n">
+        <v>110</v>
+      </c>
       <c r="O7" t="n">
-        <v>110</v>
+        <v>63.58381502890174</v>
       </c>
       <c r="P7" t="n">
-        <v>63.58381502890174</v>
+        <v>173</v>
       </c>
       <c r="Q7" t="n">
-        <v>173</v>
-      </c>
-      <c r="R7" t="n">
         <v>100</v>
       </c>
     </row>
@@ -725,10 +712,10 @@
         <v>0.8948850498428029</v>
       </c>
       <c r="F8" s="1" t="n">
-        <v>0</v>
+        <v>12.74134387819694</v>
       </c>
       <c r="G8" s="1" t="n">
-        <v>-1.064249483828396</v>
+        <v>-3.36340775681591</v>
       </c>
       <c r="H8" s="1" t="n">
         <v>6</v>
@@ -743,24 +730,21 @@
         <v>0</v>
       </c>
       <c r="L8" s="1" t="n">
-        <v>1.8</v>
+        <v>6</v>
       </c>
       <c r="M8" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="N8" s="1" t="n">
         <v>1</v>
       </c>
+      <c r="N8" t="n">
+        <v>1</v>
+      </c>
       <c r="O8" t="n">
+        <v>1.587301587301587</v>
+      </c>
+      <c r="P8" t="n">
         <v>1</v>
       </c>
-      <c r="P8" t="n">
-        <v>1.587301587301587</v>
-      </c>
       <c r="Q8" t="n">
-        <v>1</v>
-      </c>
-      <c r="R8" t="n">
         <v>1.587301587301587</v>
       </c>
     </row>
@@ -777,9 +761,11 @@
       <c r="J9" s="1" t="n"/>
       <c r="K9" s="1" t="n"/>
       <c r="L9" s="1" t="n"/>
-      <c r="M9" s="1" t="n"/>
-      <c r="N9" s="1" t="n">
+      <c r="M9" s="1" t="n">
         <v>2</v>
+      </c>
+      <c r="N9" t="n">
+        <v>0</v>
       </c>
       <c r="O9" t="n">
         <v>0</v>
@@ -788,9 +774,6 @@
         <v>0</v>
       </c>
       <c r="Q9" t="n">
-        <v>0</v>
-      </c>
-      <c r="R9" t="n">
         <v>0</v>
       </c>
     </row>
@@ -807,20 +790,19 @@
       <c r="J10" s="1" t="n"/>
       <c r="K10" s="1" t="n"/>
       <c r="L10" s="1" t="n"/>
-      <c r="M10" s="1" t="n"/>
-      <c r="N10" s="1" t="n">
+      <c r="M10" s="1" t="n">
         <v>3</v>
       </c>
+      <c r="N10" t="n">
+        <v>1</v>
+      </c>
       <c r="O10" t="n">
-        <v>1</v>
+        <v>1.587301587301587</v>
       </c>
       <c r="P10" t="n">
-        <v>1.587301587301587</v>
+        <v>2</v>
       </c>
       <c r="Q10" t="n">
-        <v>2</v>
-      </c>
-      <c r="R10" t="n">
         <v>3.174603174603174</v>
       </c>
     </row>
@@ -837,20 +819,19 @@
       <c r="J11" s="1" t="n"/>
       <c r="K11" s="1" t="n"/>
       <c r="L11" s="1" t="n"/>
-      <c r="M11" s="1" t="n"/>
-      <c r="N11" s="1" t="n">
+      <c r="M11" s="1" t="n">
         <v>4</v>
       </c>
+      <c r="N11" t="n">
+        <v>5</v>
+      </c>
       <c r="O11" t="n">
-        <v>5</v>
+        <v>7.936507936507936</v>
       </c>
       <c r="P11" t="n">
-        <v>7.936507936507936</v>
+        <v>7</v>
       </c>
       <c r="Q11" t="n">
-        <v>7</v>
-      </c>
-      <c r="R11" t="n">
         <v>11.11111111111111</v>
       </c>
     </row>
@@ -867,20 +848,19 @@
       <c r="J12" s="1" t="n"/>
       <c r="K12" s="1" t="n"/>
       <c r="L12" s="1" t="n"/>
-      <c r="M12" s="1" t="n"/>
-      <c r="N12" s="1" t="n">
+      <c r="M12" s="1" t="n">
         <v>5</v>
       </c>
+      <c r="N12" t="n">
+        <v>2</v>
+      </c>
       <c r="O12" t="n">
-        <v>2</v>
+        <v>3.174603174603174</v>
       </c>
       <c r="P12" t="n">
-        <v>3.174603174603174</v>
+        <v>9</v>
       </c>
       <c r="Q12" t="n">
-        <v>9</v>
-      </c>
-      <c r="R12" t="n">
         <v>14.28571428571428</v>
       </c>
     </row>
@@ -897,25 +877,24 @@
       <c r="J13" s="1" t="n"/>
       <c r="K13" s="1" t="n"/>
       <c r="L13" s="1" t="n"/>
-      <c r="M13" s="1" t="n"/>
-      <c r="N13" s="1" t="n">
+      <c r="M13" s="1" t="n">
         <v>6</v>
       </c>
+      <c r="N13" t="n">
+        <v>54</v>
+      </c>
       <c r="O13" t="n">
-        <v>54</v>
+        <v>85.71428571428571</v>
       </c>
       <c r="P13" t="n">
-        <v>85.71428571428571</v>
+        <v>63</v>
       </c>
       <c r="Q13" t="n">
-        <v>63</v>
-      </c>
-      <c r="R13" t="n">
         <v>100</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="25">
+  <mergeCells count="23">
     <mergeCell ref="A2:A13"/>
     <mergeCell ref="B2:B7"/>
     <mergeCell ref="B8:B13"/>
@@ -939,8 +918,6 @@
     <mergeCell ref="K8:K13"/>
     <mergeCell ref="L2:L7"/>
     <mergeCell ref="L8:L13"/>
-    <mergeCell ref="M2:M7"/>
-    <mergeCell ref="M8:M13"/>
   </mergeCells>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>